<commit_message>
Your commit message describing the changes
</commit_message>
<xml_diff>
--- a/Gantt chant.xlsx
+++ b/Gantt chant.xlsx
@@ -4,12 +4,25 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="27945" windowHeight="12330"/>
+    <workbookView windowWidth="28800" windowHeight="12300"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -43,7 +56,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
   <numFmts count="5">
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
@@ -662,14 +675,11 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="58" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -967,7 +977,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:autoTitleDeleted val="0"/>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
@@ -1020,15 +1030,15 @@
             <c:numRef>
               <c:f>Sheet1!$B$4:$B$6</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>45366</c:v>
                 </c:pt>
-                <c:pt idx="1" c:formatCode="m/d/yyyy">
+                <c:pt idx="1">
                   <c:v>45413</c:v>
                 </c:pt>
-                <c:pt idx="2" c:formatCode="m/d/yyyy">
+                <c:pt idx="2">
                   <c:v>45474</c:v>
                 </c:pt>
               </c:numCache>
@@ -2103,7 +2113,7 @@
   <dimension ref="A2:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="5" outlineLevelCol="6"/>
@@ -2140,24 +2150,24 @@
       <c r="B4" s="2">
         <v>45366</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="2">
         <v>45412</v>
       </c>
       <c r="D4">
         <f>C4-B4</f>
         <v>46</v>
       </c>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5" s="2">
         <v>45413</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="2">
         <v>45473</v>
       </c>
       <c r="D5">
@@ -2169,10 +2179,10 @@
       <c r="A6" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B6" s="2">
         <v>45474</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="2">
         <v>45519</v>
       </c>
       <c r="D6">

</xml_diff>